<commit_message>
Revert "removing _new.xlsx in the databases"
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/SUPPLY.xlsx
+++ b/cea/databases/CH/assemblies/SUPPLY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB2C5F3-0B9A-1048-96B2-6097B17971D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED9172-88B2-478F-A025-9E665100A512}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="29560" windowWidth="29040" windowHeight="18880" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="22" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -305,48 +305,6 @@
   </si>
   <si>
     <t>COOLING</t>
-  </si>
-  <si>
-    <t>primary_components</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>BO2</t>
-  </si>
-  <si>
-    <t>BO4</t>
-  </si>
-  <si>
-    <t>BO1</t>
-  </si>
-  <si>
-    <t>BO5</t>
-  </si>
-  <si>
-    <t>BO6</t>
-  </si>
-  <si>
-    <t>HP1</t>
-  </si>
-  <si>
-    <t>HP3</t>
-  </si>
-  <si>
-    <t>HP2</t>
-  </si>
-  <si>
-    <t>secondary_components</t>
-  </si>
-  <si>
-    <t>tertiary_components</t>
-  </si>
-  <si>
-    <t>CH2</t>
-  </si>
-  <si>
-    <t>CT1</t>
   </si>
 </sst>
 </file>
@@ -507,20 +465,20 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,27 +923,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="51.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -993,528 +950,411 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="J2" s="10">
-        <v>20</v>
-      </c>
-      <c r="K2" s="10">
-        <v>1</v>
-      </c>
-      <c r="L2" s="10">
-        <v>5</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G2" s="10">
+        <v>20</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6">
+      <c r="E3" s="6">
         <v>0.8</v>
       </c>
-      <c r="I3" s="6">
+      <c r="F3" s="6">
         <v>493</v>
       </c>
-      <c r="J3" s="10">
-        <v>20</v>
-      </c>
-      <c r="K3" s="10">
-        <v>1</v>
-      </c>
-      <c r="L3" s="10">
-        <v>5</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="G3" s="10">
+        <v>20</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="6">
+      <c r="E4" s="6">
         <v>0.6</v>
       </c>
-      <c r="I4" s="6">
+      <c r="F4" s="6">
         <v>367</v>
       </c>
-      <c r="J4" s="10">
-        <v>20</v>
-      </c>
-      <c r="K4" s="10">
-        <v>1</v>
-      </c>
-      <c r="L4" s="10">
-        <v>5</v>
-      </c>
-      <c r="M4" s="9" t="s">
+      <c r="G4" s="10">
+        <v>20</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>5</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="6">
+      <c r="E5" s="6">
         <v>0.8</v>
       </c>
-      <c r="I5" s="6">
+      <c r="F5" s="6">
         <v>645</v>
       </c>
-      <c r="J5" s="10">
-        <v>20</v>
-      </c>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10">
-        <v>5</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="G5" s="10">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
+        <v>5</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="6">
+      <c r="E6" s="6">
         <v>0.9</v>
       </c>
-      <c r="I6" s="6">
+      <c r="F6" s="6">
         <v>200</v>
       </c>
-      <c r="J6" s="10">
-        <v>20</v>
-      </c>
-      <c r="K6" s="10">
-        <v>1</v>
-      </c>
-      <c r="L6" s="10">
-        <v>5</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G6" s="10">
+        <v>20</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="6">
+      <c r="E7" s="6">
         <v>0.6</v>
       </c>
-      <c r="I7" s="6">
+      <c r="F7" s="6">
         <v>200</v>
       </c>
-      <c r="J7" s="10">
-        <v>20</v>
-      </c>
-      <c r="K7" s="10">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10">
-        <v>5</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G7" s="10">
+        <v>20</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="6">
+      <c r="E8" s="6">
         <v>4</v>
       </c>
-      <c r="I8" s="6">
+      <c r="F8" s="6">
         <v>200</v>
       </c>
-      <c r="J8" s="10">
-        <v>20</v>
-      </c>
-      <c r="K8" s="10">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10">
-        <v>5</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G8" s="10">
+        <v>20</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="6">
+      <c r="E9" s="6">
         <v>2.7</v>
       </c>
-      <c r="I9" s="6">
+      <c r="F9" s="6">
         <v>200</v>
       </c>
-      <c r="J9" s="10">
-        <v>20</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10">
-        <v>5</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G9" s="10">
+        <v>20</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10">
+        <v>5</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="6">
+      <c r="E10" s="6">
         <v>3</v>
       </c>
-      <c r="I10" s="6">
+      <c r="F10" s="6">
         <v>200</v>
       </c>
-      <c r="J10" s="10">
-        <v>20</v>
-      </c>
-      <c r="K10" s="10">
-        <v>1</v>
-      </c>
-      <c r="L10" s="10">
-        <v>5</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" s="10">
+        <v>20</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>5</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="6">
+      <c r="E11" s="6">
         <v>0.6</v>
       </c>
-      <c r="I11" s="6">
+      <c r="F11" s="6">
         <v>100</v>
       </c>
-      <c r="J11" s="10">
-        <v>20</v>
-      </c>
-      <c r="K11" s="10">
-        <v>1</v>
-      </c>
-      <c r="L11" s="10">
-        <v>5</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G11" s="10">
+        <v>20</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="6">
+      <c r="E12" s="6">
         <v>3</v>
       </c>
-      <c r="I12" s="6">
+      <c r="F12" s="6">
         <v>100</v>
       </c>
-      <c r="J12" s="10">
-        <v>20</v>
-      </c>
-      <c r="K12" s="10">
-        <v>1</v>
-      </c>
-      <c r="L12" s="10">
-        <v>5</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G12" s="10">
+        <v>20</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>5</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="6">
+      <c r="E13" s="6">
         <v>2.7</v>
       </c>
-      <c r="I13" s="6">
+      <c r="F13" s="6">
         <v>100</v>
       </c>
-      <c r="J13" s="10">
-        <v>20</v>
-      </c>
-      <c r="K13" s="10">
-        <v>1</v>
-      </c>
-      <c r="L13" s="10">
-        <v>5</v>
-      </c>
-      <c r="M13" s="5" t="s">
+      <c r="G13" s="10">
+        <v>20</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="10">
+        <v>5</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1532,20 +1372,20 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="51.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1577,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1641,7 +1481,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
@@ -1705,7 +1545,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1737,7 +1577,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1769,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1801,7 +1641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1833,7 +1673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1865,7 +1705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1897,7 +1737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
@@ -1929,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
@@ -1969,27 +1809,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" customWidth="1"/>
+    <col min="11" max="11" width="51.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1997,43 +1837,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2041,43 +1872,34 @@
         <v>60</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="J2" s="4">
+      <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="K2" s="10">
-        <v>20</v>
-      </c>
-      <c r="L2" s="10">
-        <v>1</v>
-      </c>
-      <c r="M2" s="10">
-        <v>5</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H2" s="10">
+        <v>20</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>5</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
@@ -2085,43 +1907,34 @@
         <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6">
+      <c r="F3" s="6">
         <v>2.7</v>
       </c>
-      <c r="J3" s="6">
+      <c r="G3" s="6">
         <v>200</v>
       </c>
-      <c r="K3" s="10">
-        <v>20</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1</v>
-      </c>
-      <c r="M3" s="10">
-        <v>5</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H3" s="10">
+        <v>20</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10">
+        <v>5</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -2129,43 +1942,34 @@
         <v>62</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="6">
+      <c r="F4" s="6">
         <v>3</v>
       </c>
-      <c r="J4" s="6">
+      <c r="G4" s="6">
         <v>200</v>
       </c>
-      <c r="K4" s="10">
-        <v>20</v>
-      </c>
-      <c r="L4" s="10">
-        <v>1</v>
-      </c>
-      <c r="M4" s="10">
-        <v>5</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H4" s="10">
+        <v>20</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>5</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -2173,43 +1977,34 @@
         <v>63</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3">
+      <c r="F5" s="3">
         <v>3.2</v>
       </c>
-      <c r="J5" s="6">
+      <c r="G5" s="6">
         <v>200</v>
       </c>
-      <c r="K5" s="10">
-        <v>20</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="10">
-        <v>5</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H5" s="10">
+        <v>20</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -2217,39 +2012,30 @@
         <v>64</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="5">
+      <c r="F6" s="5">
         <v>2.8</v>
       </c>
-      <c r="J6" s="6">
+      <c r="G6" s="6">
         <v>200</v>
       </c>
-      <c r="K6" s="10">
-        <v>20</v>
-      </c>
-      <c r="L6" s="10">
-        <v>1</v>
-      </c>
-      <c r="M6" s="10">
-        <v>5</v>
-      </c>
-      <c r="N6" s="5" t="s">
+      <c r="H6" s="10">
+        <v>20</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
+        <v>5</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2262,24 +2048,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="51.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2311,7 +2097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2343,7 +2129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>

</xml_diff>